<commit_message>
Add .env to gitignore
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -7,9 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SES案件一覧" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SES案件一覧'!$A$1:$G$8</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -17,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,13 +27,22 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFACD"/>
+        <bgColor rgb="00FFFACD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +57,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,163 +430,297 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="33" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="29" customWidth="1" min="5" max="5"/>
+    <col width="27" customWidth="1" min="6" max="6"/>
+    <col width="29" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="20" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>案件名</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>作業内容</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>募集要件</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>募集人数</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>期間</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>勤務場所</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>その他</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>受注管理システムの運用保守・問合せ対応・EDI関連の保守対応</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>・受注管理システムの運用保守　・問合せに対する調査対応　・EDI関連の保守業務</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>SQLの実務経験（※特に優先）日本語での高度な理解・会話力（流暢）（※特に優先）</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>未記入</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024年7月〜（長期想定）</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>仙川（出社対応あり）</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>未記入</t>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>EBS導入支援</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>購買管理システムの維持・保守対応（改修・テスト等）</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Java、PL/SQL開発経験（5年以上）、テスト仕様書の作成および実施経験</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>1名</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>2025/7/1～2025/7/31　◎継続有り</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>リモート</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>単価：～65万円、月固定</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DX関連開発案件（アジャイル開発）</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>基本設計～製造・テスト</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Python開発経験</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1～2名</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7月開始予定</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>御茶ノ水（リモート相談可）</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>未記入</t>
+    <row r="3" ht="30" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>スマホアプリ開発</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>iOS(Swift)アプリの開発経験のある方(3年以上)、設計～実装～評価</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>日本語流暢、object-c経験あれば、ベスト,flutter、主体的に業務推進できること</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr"/>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>2025/6～長期できる方</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr"/>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>単金：MAX63万円、貴社まで</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>某業界向けSAP UI5開発</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>UI5での画面新規作成</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>・UI5での開発経験</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>１名</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>7月～9月末予定（延長、または他案件シフトあり）</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>虎ノ門</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>現場の勤務時間に従い、</t>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>カメラファームウェア開発</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr"/>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>組込みC/C++5年以上経験、日本語N1流暢</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr"/>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>2025/7/1～(2年以上対応可能な方のみ)</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>横浜周辺出勤</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>単金：MAX65、貴社まで、SET可能です。</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>SAS分析モデルの追加開発など、複数案件</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>SAS、DWHシステムの構築を行うSASの設計、開発、テストを実施予定。</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>SAS基盤構築経験、詳細設計以降の開発経験、データパイプライン構築経験、日本語流暢</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>複数名</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>2025/7～</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>都内常駐</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr"/>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>大阪の銀行システム移行支援</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>cobol　or JAVA設計・開発できるの方</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>6-10人</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>即日～二年予定</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>大阪</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>大阪に在住の日本人を募集しています。</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="45" customHeight="1">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>通信キャリア様向けネットワーク構築PJのPMサポート業務</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>エンジニアの作業サポート(海外-日本間の通訳、PMからの指示の伝達等)、会議でのプロジェクトの進捗報告、課題管理、資料・議事録作成、プロジェクトの工程管理・調整、顧客との協議、QA対応、海外R&amp;Dとの会議</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>英語での読み書き、英会話ができること、能動的にコミュニケーションが取れること、基地局やOSSなどモバイルシステムに関する基本知識や実務経験があること、プロジェクトサポート業務の経験があること</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>1名</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>2025/7/1～2025/12/31</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>川崎、六本木オフィス、顧客ラボ(豊洲、多摩)</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>45万円～50万円(固定) ※経験値により応相談</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>オープン系COBOL</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>基本設計～テスト</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>DB（ORACLE）、SQL、shell</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>3名</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>7月から</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>出社必須</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>入社限定</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G8"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>